<commit_message>
Merged PR 34: HorizonDialogue Demo
Related work items: #432, #507, #509, #536, #548
</commit_message>
<xml_diff>
--- a/DesignerRawData/Excel/Test.xlsx
+++ b/DesignerRawData/Excel/Test.xlsx
@@ -1,22 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3115D9BC-BD79-421F-8CCA-183BBBD99701}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7620BC1C-7EA9-4C30-B891-B84F7218A0FF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="DT_Test_Title" sheetId="2" r:id="rId1"/>
-    <sheet name="DT_Test_Content" sheetId="1" r:id="rId2"/>
+    <sheet name="TestTitle_StringTable" sheetId="1" r:id="rId1"/>
+    <sheet name="TestContent_StringTable" sheetId="2" r:id="rId2"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId3"/>
-  </externalReferences>
-  <definedNames>
-    <definedName name="DialogueTalkerName.xlsx">[1]!DialogueTalkerNameID</definedName>
-  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -27,37 +21,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
-  <si>
-    <t>id_001</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+  <si>
+    <t>Key</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>DialogueText</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DialogueTalkerNameID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>SourceString</t>
+  </si>
+  <si>
+    <t>Comment</t>
   </si>
   <si>
     <t>id_000</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>id_003</t>
-  </si>
-  <si>
-    <t>id_004</t>
-  </si>
-  <si>
-    <t>id_005</t>
-  </si>
-  <si>
-    <t>id_006</t>
-  </si>
-  <si>
-    <t>id_007</t>
+    <t>Long Dialogue Test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Test Message1</t>
@@ -86,15 +67,8 @@
     <t>Test Message8</t>
   </si>
   <si>
-    <t>id_002</t>
-  </si>
-  <si>
-    <t>id_long_rich_test</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">&lt;text color="#77FF77AA" shadowColor="#FF0000FF" shadowOffset="[4,3]"&gt;This is rich text simple test:&lt;/text&gt;&lt;br/&gt;
-&lt;text color="#FF0000AA"&gt;This is programmer:&lt;/text&gt;&lt;img filePath="PaperSprite'/Game/HorizonUIDemo/SpriteSheet/Test/Frames/programmer_png.programmer_png'" size="[50, 50]" /&gt;&lt;br/&gt;
+&lt;text color="#FF0000AA"&gt;This is programmer:&lt;/text&gt;&lt;img filePath="PaperSprite'/Game/HorizonDialogueDemo/Textures/Character/programmer_Sprite.programmer_Sprite'" size="[50, 50]" /&gt;&lt;br/&gt;
 &lt;text color="#0000FFFF"&gt;This is a WaterMellon:&lt;/text&gt;&lt;img color="#FF00FF77" filePath="PaperSprite'/Game/HorizonUIDemo/SpriteSheet/Test/Frames/I_C_Watermellon_png.I_C_Watermellon_png'" size="[50, 50]" /&gt; &lt;br/&gt;
 &lt;text color="#77FF77AA" shadowColor="#FF0000FF" shadowOffset="[4,3]"&gt;This is rich text simple test:&lt;/text&gt;&lt;br/&gt;
 &lt;text&gt;Test Message 1234578910111213141516171819&lt;/text&gt;&lt;br/&gt;
@@ -146,11 +120,28 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>id_test</t>
-  </si>
-  <si>
-    <t>Long Dialogue Test</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>id_001</t>
+  </si>
+  <si>
+    <t>id_002</t>
+  </si>
+  <si>
+    <t>id_003</t>
+  </si>
+  <si>
+    <t>id_004</t>
+  </si>
+  <si>
+    <t>id_005</t>
+  </si>
+  <si>
+    <t>id_006</t>
+  </si>
+  <si>
+    <t>id_007</t>
+  </si>
+  <si>
+    <t>id_008</t>
   </si>
 </sst>
 </file>
@@ -213,28 +204,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="DialogueTalkerName"/>
-    </sheetNames>
-    <definedNames>
-      <definedName name="DialogueTalkerNameID" refersTo="='DialogueTalkerName'!$A:$A"/>
-    </definedNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="2">
-          <cell r="A2" t="str">
-            <v>id_programmer</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -499,67 +468,62 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D944F81E-5369-42AC-AE8C-300297A3D42E}">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45D91AD8-BBA2-417E-ABD4-9055FB5A823F}">
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.42578125" customWidth="1"/>
-    <col min="2" max="2" width="40.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="1">
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="A1" xr:uid="{1E7EC4AB-D541-4165-B09A-CF782ABF7DCD}"/>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C10"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="22.7109375" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="3" max="3" width="92.85546875" customWidth="1"/>
-    <col min="4" max="4" width="62.7109375" customWidth="1"/>
+    <col min="2" max="2" width="36.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -567,109 +531,75 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="2">
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="B1" xr:uid="{0B193EB9-6AF1-4DB2-9D2A-921F66772904}"/>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576" xr:uid="{55CB7F29-A9B6-4F34-9917-155B665679BE}">
-      <formula1>DialogueTalkerName.xlsx</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>